<commit_message>
Bilder FEM til rapport
</commit_message>
<xml_diff>
--- a/Godkjenning for bestillingsliste/Konvergensstudie.xlsx
+++ b/Godkjenning for bestillingsliste/Konvergensstudie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uiano-my.sharepoint.com/personal/idald_uia_no/Documents/Dokumenter/MAS309/Bunnplate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uiano-my.sharepoint.com/personal/idald_uia_no/Documents/Dokumenter/MAS309/Godkjenning for bestillingsliste/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{3A6FC9A5-BE91-44BE-9FD1-316DA2D6241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F516D198-F04D-4501-B4ED-3D14456978D3}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{3A6FC9A5-BE91-44BE-9FD1-316DA2D6241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0FE270D-20BE-473F-95FE-FAD4565F4AB7}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{E9382C19-FCF0-4A75-9C16-E189F4710CB3}"/>
   </bookViews>
@@ -169,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -177,11 +177,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -214,6 +212,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nb-NO"/>
+              <a:t>Convergence</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nb-NO" baseline="0"/>
+              <a:t> study</a:t>
+            </a:r>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -366,6 +394,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Number of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nb-NO" baseline="0"/>
+                  <a:t> elements</a:t>
+                </a:r>
+                <a:endParaRPr lang="nb-NO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nb-NO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -429,6 +517,96 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Max von Mises stress</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nb-NO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1440,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11791004-8BF7-423E-AA9A-135A9BB01244}">
-  <dimension ref="A2:H14"/>
+  <dimension ref="A2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1454,101 +1632,58 @@
     <col min="7" max="7" width="14.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6" s="3">
         <v>6372</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="4">
         <v>168</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7" s="3">
         <v>7078</v>
       </c>
       <c r="C7" s="4">
         <v>169</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8" s="3">
         <v>9466</v>
       </c>
       <c r="C8" s="4">
         <v>168</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" s="5">
         <v>14534</v>
       </c>
       <c r="C9" s="6">
         <v>170</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>